<commit_message>
Finalizada a parte do banco de dados
</commit_message>
<xml_diff>
--- a/BancoDeDados-Sprint1/modelagens/SP-Medical-Group-SPMedicalGroup-fisico.xlsx
+++ b/BancoDeDados-Sprint1/modelagens/SP-Medical-Group-SPMedicalGroup-fisico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fic\Desktop\SPMedicalGroup\BancoDeDados-Sprint1\modelagens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9891735-EB15-48FA-B994-2E8B399BAC7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32363446-8010-48D3-9593-1AA89C79C22C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{342AA421-BF79-47DC-AAD9-CF023D4EA105}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="122">
   <si>
     <t>especialidade</t>
   </si>
@@ -144,9 +144,6 @@
     <t>idUsuario</t>
   </si>
   <si>
-    <t>nome</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -247,13 +244,160 @@
   </si>
   <si>
     <t>ric123</t>
+  </si>
+  <si>
+    <t>medico</t>
+  </si>
+  <si>
+    <t>idMedico</t>
+  </si>
+  <si>
+    <t>crm</t>
+  </si>
+  <si>
+    <t>54356-SP</t>
+  </si>
+  <si>
+    <t>53452-SP</t>
+  </si>
+  <si>
+    <t>65463-SP</t>
+  </si>
+  <si>
+    <t>paciente</t>
+  </si>
+  <si>
+    <t>idPaciente</t>
+  </si>
+  <si>
+    <t>dataNascimento</t>
+  </si>
+  <si>
+    <t>telefone</t>
+  </si>
+  <si>
+    <t>rg</t>
+  </si>
+  <si>
+    <t>cpf</t>
+  </si>
+  <si>
+    <t>enderecoPaciente</t>
+  </si>
+  <si>
+    <t>11 3456-7654</t>
+  </si>
+  <si>
+    <t>11 98765-6543</t>
+  </si>
+  <si>
+    <t>11 97208-4453</t>
+  </si>
+  <si>
+    <t>11 3456-6543</t>
+  </si>
+  <si>
+    <t>11 7656-6377</t>
+  </si>
+  <si>
+    <t>11 95436-8769</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>43522543-5</t>
+  </si>
+  <si>
+    <t>32654345-7</t>
+  </si>
+  <si>
+    <t>54636525-3</t>
+  </si>
+  <si>
+    <t>54366362-5</t>
+  </si>
+  <si>
+    <t>t32544444-1</t>
+  </si>
+  <si>
+    <t>54566266-7</t>
+  </si>
+  <si>
+    <t>54566266-8</t>
+  </si>
+  <si>
+    <t>Rua Estado de Israel 240, São Paulo, Estado de São Paulo, 04022-000</t>
+  </si>
+  <si>
+    <t>Av. Paulista, 1578 - Bela Vista, São Paulo - SP, 01310-200</t>
+  </si>
+  <si>
+    <t>Av. Ibirapuera - Indianópolis, 2927,  São Paulo - SP, 04029-200</t>
+  </si>
+  <si>
+    <t>R. Vitória, 120 - Vila Sao Jorge, Barueri - SP, 06402-030</t>
+  </si>
+  <si>
+    <t>R. Ver. Geraldo de Camargo, 66 - Santa Luzia, Ribeirão Pires - SP, 09405-380</t>
+  </si>
+  <si>
+    <t>Alameda dos Arapanés, 945 - Indianópolis, São Paulo - SP, 04524-001</t>
+  </si>
+  <si>
+    <t>R Sao Antonio, 232 - Vila Universal, Barueri - SP, 06407-140</t>
+  </si>
+  <si>
+    <t>situacao</t>
+  </si>
+  <si>
+    <t>idSituacao</t>
+  </si>
+  <si>
+    <t>nomeSituacao</t>
+  </si>
+  <si>
+    <t>Realizada</t>
+  </si>
+  <si>
+    <t>Agendada</t>
+  </si>
+  <si>
+    <t>Cancelada</t>
+  </si>
+  <si>
+    <t>consulta</t>
+  </si>
+  <si>
+    <t>idConsulta</t>
+  </si>
+  <si>
+    <t>dataConsulta</t>
+  </si>
+  <si>
+    <t>descricaoConsulta</t>
+  </si>
+  <si>
+    <t>Consulta realizada com sucesso.</t>
+  </si>
+  <si>
+    <t>Consulta cancelada com sucesso.</t>
+  </si>
+  <si>
+    <t>Consulta agendada com sucesso.</t>
+  </si>
+  <si>
+    <t>nomePaciente</t>
+  </si>
+  <si>
+    <t>nomeMedico</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,8 +413,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,8 +501,80 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -465,22 +689,78 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -499,27 +779,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -532,15 +797,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -551,15 +807,216 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="19" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="19" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="19" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="22" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="22" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -569,6 +1026,20 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCFF"/>
+      <color rgb="FFFF99FF"/>
+      <color rgb="FF00FFFF"/>
+      <color rgb="FF66FFFF"/>
+      <color rgb="FF33CCCC"/>
+      <color rgb="FFCCFFFF"/>
+      <color rgb="FFFFFFCC"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFFFFF66"/>
+      <color rgb="FFFF66FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -877,120 +1348,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F098C7-5494-4F6C-B2E4-16358E9D3F59}">
-  <dimension ref="B1:Q22"/>
+  <dimension ref="B1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.21875" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" customWidth="1"/>
-    <col min="11" max="11" width="32.5546875" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+    <col min="11" max="11" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="67.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.77734375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="E2" s="10" t="s">
+      <c r="C2" s="71"/>
+      <c r="E2" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="12"/>
-      <c r="M2" s="15" t="s">
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="16"/>
-    </row>
-    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="N2" s="76"/>
+    </row>
+    <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="R3" s="86"/>
+    </row>
+    <row r="4" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="14">
-        <v>1</v>
-      </c>
-      <c r="F4" s="9" t="s">
+      <c r="E4" s="9">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="14" t="s">
+      <c r="G4" s="83">
+        <v>0.3125</v>
+      </c>
+      <c r="H4" s="84">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="18">
-        <v>1</v>
-      </c>
-      <c r="N4" s="18" t="s">
+      <c r="M4" s="11">
+        <v>1</v>
+      </c>
+      <c r="N4" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="5">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="1"/>
@@ -1000,18 +1479,18 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="M5" s="19">
+      <c r="M5" s="12">
         <v>2</v>
       </c>
-      <c r="N5" s="19" t="s">
+      <c r="N5" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="5">
+    <row r="6" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="1"/>
@@ -1020,346 +1499,789 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="M6" s="20">
+      <c r="K6" s="85"/>
+      <c r="M6" s="13">
         <v>3</v>
       </c>
-      <c r="N6" s="20" t="s">
+      <c r="N6" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="5">
+    <row r="7" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="5">
+      <c r="F7" s="80" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="81"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="89"/>
+      <c r="Q7" s="18"/>
+    </row>
+    <row r="8" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="3">
         <v>5</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="M8" s="21" t="s">
+      <c r="F8" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="23"/>
-    </row>
-    <row r="9" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="5">
+      <c r="N8" s="78"/>
+      <c r="O8" s="78"/>
+      <c r="P8" s="79"/>
+      <c r="Q8" s="88"/>
+      <c r="R8" s="18"/>
+    </row>
+    <row r="9" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="3">
         <v>6</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="24" t="s">
+      <c r="F9" s="21">
+        <v>1</v>
+      </c>
+      <c r="G9" s="90" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="27">
+        <v>1</v>
+      </c>
+      <c r="I9" s="22">
+        <v>1</v>
+      </c>
+      <c r="J9" s="27">
+        <v>2</v>
+      </c>
+      <c r="K9" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="M9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="N9" s="24" t="s">
+      <c r="N9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="O9" s="24" t="s">
+      <c r="O9" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="P9" s="24" t="s">
+      <c r="P9" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="Q9" s="24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="5">
+      <c r="Q9" s="87"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
         <v>7</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M10" s="25">
-        <v>1</v>
-      </c>
-      <c r="N10" s="25">
+      <c r="F10" s="21">
         <v>2</v>
       </c>
-      <c r="O10" s="25" t="s">
+      <c r="G10" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="P10" s="25" t="s">
+      <c r="H10" s="27">
+        <v>2</v>
+      </c>
+      <c r="I10" s="22">
+        <v>1</v>
+      </c>
+      <c r="J10" s="27">
+        <v>17</v>
+      </c>
+      <c r="K10" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="M10" s="15">
+        <v>1</v>
+      </c>
+      <c r="N10" s="15">
+        <v>2</v>
+      </c>
+      <c r="O10" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="P10" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="3">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="24">
+        <v>3</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="28">
+        <v>3</v>
+      </c>
+      <c r="I11" s="25">
+        <v>1</v>
+      </c>
+      <c r="J11" s="28">
+        <v>16</v>
+      </c>
+      <c r="K11" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="M11" s="15">
+        <v>2</v>
+      </c>
+      <c r="N11" s="15">
+        <v>2</v>
+      </c>
+      <c r="O11" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="Q10" s="25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="5">
+      <c r="P11" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="3">
+        <v>9</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="M12" s="15">
+        <v>3</v>
+      </c>
+      <c r="N12" s="15">
+        <v>2</v>
+      </c>
+      <c r="O12" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="P12" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="3">
+        <v>10</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="64"/>
+      <c r="M13" s="15">
+        <v>4</v>
+      </c>
+      <c r="N13" s="15">
+        <v>1</v>
+      </c>
+      <c r="O13" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="P13" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="3">
+        <v>11</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="H14" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="I14" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="J14" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="K14" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="L14" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="M14" s="15">
+        <v>5</v>
+      </c>
+      <c r="N14" s="15">
+        <v>1</v>
+      </c>
+      <c r="O14" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="P14" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <v>12</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="34">
+        <v>1</v>
+      </c>
+      <c r="F15" s="39">
+        <v>4</v>
+      </c>
+      <c r="G15" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="40">
+        <v>30602</v>
+      </c>
+      <c r="I15" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="J15" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="K15" s="39">
+        <v>94839859000</v>
+      </c>
+      <c r="L15" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="M15" s="15">
+        <v>6</v>
+      </c>
+      <c r="N15" s="15">
+        <v>1</v>
+      </c>
+      <c r="O15" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="P15" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B16" s="3">
+        <v>13</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="34">
+        <v>2</v>
+      </c>
+      <c r="F16" s="34">
+        <v>5</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="43">
+        <v>37095</v>
+      </c>
+      <c r="I16" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="J16" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="K16" s="34">
+        <v>73556944057</v>
+      </c>
+      <c r="L16" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="M16" s="15">
+        <v>7</v>
+      </c>
+      <c r="N16" s="15">
+        <v>1</v>
+      </c>
+      <c r="O16" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="P16" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B17" s="3">
+        <v>14</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="34">
+        <v>3</v>
+      </c>
+      <c r="F17" s="34">
+        <v>6</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="43">
+        <v>28773</v>
+      </c>
+      <c r="I17" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="J17" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="K17" s="34">
+        <v>16839338002</v>
+      </c>
+      <c r="L17" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="M17" s="15">
         <v>8</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="N17" s="15">
+        <v>1</v>
+      </c>
+      <c r="O17" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="P17" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B18" s="3">
+        <v>15</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="34">
+        <v>4</v>
+      </c>
+      <c r="F18" s="34">
+        <v>7</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="43">
+        <v>31333</v>
+      </c>
+      <c r="I18" s="91" t="s">
+        <v>89</v>
+      </c>
+      <c r="J18" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="K18" s="34">
+        <v>14332654765</v>
+      </c>
+      <c r="L18" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="M18" s="15">
+        <v>9</v>
+      </c>
+      <c r="N18" s="15">
+        <v>1</v>
+      </c>
+      <c r="O18" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="P18" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B19" s="3">
+        <v>16</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="34">
+        <v>5</v>
+      </c>
+      <c r="F19" s="34">
+        <v>8</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="43">
+        <v>27633</v>
+      </c>
+      <c r="I19" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="J19" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="K19" s="34">
+        <v>91305348010</v>
+      </c>
+      <c r="L19" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="M19" s="15">
         <v>10</v>
       </c>
-      <c r="M11" s="25">
+      <c r="N19" s="15">
+        <v>1</v>
+      </c>
+      <c r="O19" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="P19" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="20">
+        <v>17</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="34">
+        <v>6</v>
+      </c>
+      <c r="F20" s="34">
+        <v>9</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="43">
+        <v>26379</v>
+      </c>
+      <c r="I20" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="J20" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="K20" s="34">
+        <v>79799299004</v>
+      </c>
+      <c r="L20" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="M20" s="16">
+        <v>11</v>
+      </c>
+      <c r="N20" s="16">
+        <v>3</v>
+      </c>
+      <c r="O20" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="P20" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="35">
+        <v>7</v>
+      </c>
+      <c r="F21" s="35">
+        <v>10</v>
+      </c>
+      <c r="G21" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" s="45">
+        <v>43164</v>
+      </c>
+      <c r="I21" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="J21" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="K21" s="35">
+        <v>13771913039</v>
+      </c>
+      <c r="L21" s="47" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C22" s="18"/>
+    </row>
+    <row r="25" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G26" s="67" t="s">
+        <v>113</v>
+      </c>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="68"/>
+      <c r="K26" s="68"/>
+      <c r="L26" s="69"/>
+    </row>
+    <row r="27" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G27" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="H27" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="I27" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="J27" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="K27" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="L27" s="49" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="66"/>
+      <c r="G28" s="51">
+        <v>1</v>
+      </c>
+      <c r="H28" s="52">
+        <v>7</v>
+      </c>
+      <c r="I28" s="53">
+        <v>3</v>
+      </c>
+      <c r="J28" s="52">
+        <v>1</v>
+      </c>
+      <c r="K28" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="L28" s="54">
+        <v>43850.625</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="59" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="G29" s="51">
         <v>2</v>
       </c>
-      <c r="N11" s="25">
+      <c r="H29" s="52">
         <v>2</v>
       </c>
-      <c r="O11" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="P11" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q11" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="5">
-        <v>9</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" s="25">
+      <c r="I29" s="53">
+        <v>2</v>
+      </c>
+      <c r="J29" s="52">
         <v>3</v>
       </c>
-      <c r="N12" s="25">
+      <c r="K29" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="L29" s="54">
+        <v>43836.416666666664</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B30" s="60">
+        <v>1</v>
+      </c>
+      <c r="C30" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="G30" s="51">
+        <v>3</v>
+      </c>
+      <c r="H30" s="52">
+        <v>3</v>
+      </c>
+      <c r="I30" s="53">
         <v>2</v>
       </c>
-      <c r="O12" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="P12" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q12" s="25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="5">
-        <v>10</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="M13" s="25">
+      <c r="J30" s="52">
+        <v>1</v>
+      </c>
+      <c r="K30" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="L30" s="54">
+        <v>43868.458333333336</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B31" s="60">
+        <v>2</v>
+      </c>
+      <c r="C31" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="G31" s="51">
         <v>4</v>
       </c>
-      <c r="N13" s="25">
-        <v>1</v>
-      </c>
-      <c r="O13" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="P13" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q13" s="25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="5">
-        <v>11</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="M14" s="25">
+      <c r="H31" s="52">
+        <v>2</v>
+      </c>
+      <c r="I31" s="53">
+        <v>2</v>
+      </c>
+      <c r="J31" s="52">
+        <v>1</v>
+      </c>
+      <c r="K31" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="L31" s="54">
+        <v>43137.416666666664</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="61">
+        <v>3</v>
+      </c>
+      <c r="C32" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="G32" s="51">
         <v>5</v>
       </c>
-      <c r="N14" s="25">
-        <v>1</v>
-      </c>
-      <c r="O14" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="P14" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q14" s="25" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="5">
-        <v>12</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M15" s="25">
+      <c r="H32" s="52">
+        <v>4</v>
+      </c>
+      <c r="I32" s="53">
+        <v>1</v>
+      </c>
+      <c r="J32" s="52">
+        <v>3</v>
+      </c>
+      <c r="K32" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="L32" s="54">
+        <v>43503.458333333336</v>
+      </c>
+    </row>
+    <row r="33" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G33" s="51">
         <v>6</v>
       </c>
-      <c r="N15" s="25">
-        <v>1</v>
-      </c>
-      <c r="O15" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="P15" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q15" s="25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="5">
-        <v>13</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="30"/>
-      <c r="M16" s="25">
+      <c r="H33" s="52">
         <v>7</v>
       </c>
-      <c r="N16" s="25">
-        <v>1</v>
-      </c>
-      <c r="O16" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="P16" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q16" s="25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B17" s="5">
-        <v>14</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M17" s="25">
-        <v>8</v>
-      </c>
-      <c r="N17" s="25">
-        <v>1</v>
-      </c>
-      <c r="O17" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="P17" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q17" s="25" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B18" s="5">
-        <v>15</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K18" s="30"/>
-      <c r="M18" s="25">
-        <v>9</v>
-      </c>
-      <c r="N18" s="25">
-        <v>1</v>
-      </c>
-      <c r="O18" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="P18" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q18" s="25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B19" s="5">
-        <v>16</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M19" s="25">
-        <v>10</v>
-      </c>
-      <c r="N19" s="25">
-        <v>1</v>
-      </c>
-      <c r="O19" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="P19" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q19" s="25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="32">
-        <v>17</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="M20" s="26">
-        <v>11</v>
-      </c>
-      <c r="N20" s="26">
+      <c r="I33" s="53">
         <v>3</v>
       </c>
-      <c r="O20" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="P20" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q20" s="26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="30"/>
-      <c r="P21" s="29"/>
-      <c r="Q21" s="28"/>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="C22" s="30"/>
+      <c r="J33" s="52">
+        <v>2</v>
+      </c>
+      <c r="K33" s="53" t="s">
+        <v>119</v>
+      </c>
+      <c r="L33" s="54">
+        <v>43898.625</v>
+      </c>
+    </row>
+    <row r="34" spans="7:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G34" s="55">
+        <v>7</v>
+      </c>
+      <c r="H34" s="56">
+        <v>4</v>
+      </c>
+      <c r="I34" s="57">
+        <v>1</v>
+      </c>
+      <c r="J34" s="56">
+        <v>2</v>
+      </c>
+      <c r="K34" s="57" t="s">
+        <v>119</v>
+      </c>
+      <c r="L34" s="58">
+        <v>43899.458333333336</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="E13:L13"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="G26:L26"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:K2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M8:Q8"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>